<commit_message>
don't know what change
</commit_message>
<xml_diff>
--- a/IR/空调红外.xlsx
+++ b/IR/空调红外.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Develop\Code\python\My_IOT_Project\IR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{361C2DD1-31F1-4F2C-8F39-6C0FD2987762}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{237ADC92-5CC3-4477-8A43-164014517918}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7455" xr2:uid="{B469431B-2AEB-4446-856D-F9602E88A4CE}"/>
   </bookViews>
@@ -161,7 +161,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F15" authorId="0" shapeId="0" xr:uid="{CF9AC19A-6656-488E-AC38-DC8AE87A864E}">
+    <comment ref="D15" authorId="0" shapeId="0" xr:uid="{BB860E44-7497-49DF-9FB5-7239F01ECD11}">
       <text>
         <r>
           <rPr>
@@ -169,7 +169,6 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Shangbin Zhang:</t>
@@ -179,11 +178,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
-与开关有关</t>
+温度校验位，开的比关的多100</t>
         </r>
       </text>
     </comment>
@@ -343,11 +341,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -669,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAF0ABF0-B3FB-4AA2-B44A-90E1ED67786F}">
   <dimension ref="A1:AJ60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19:H30"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="X7" sqref="X7:Y9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.5" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -679,87 +677,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
+      <c r="J1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
       <c r="R1" s="1"/>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
       <c r="AA1" s="1"/>
-      <c r="AB1" s="2" t="s">
+      <c r="AB1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AC1" s="2"/>
-      <c r="AD1" s="2"/>
-      <c r="AE1" s="2"/>
-      <c r="AF1" s="2"/>
-      <c r="AG1" s="2"/>
-      <c r="AH1" s="2"/>
-      <c r="AI1" s="2"/>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
+      <c r="AE1" s="3"/>
+      <c r="AF1" s="3"/>
+      <c r="AG1" s="3"/>
+      <c r="AH1" s="3"/>
+      <c r="AI1" s="3"/>
       <c r="AJ1" s="1"/>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
       <c r="R2" s="1"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
       <c r="AA2" s="1"/>
-      <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
-      <c r="AD2" s="2"/>
-      <c r="AE2" s="2"/>
-      <c r="AF2" s="2"/>
-      <c r="AG2" s="2"/>
-      <c r="AH2" s="2"/>
-      <c r="AI2" s="2"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
+      <c r="AG2" s="3"/>
+      <c r="AH2" s="3"/>
+      <c r="AI2" s="3"/>
       <c r="AJ2" s="1"/>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.2">
@@ -870,19 +868,19 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" s="3">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0</v>
-      </c>
-      <c r="H4" s="3">
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
         <v>1</v>
       </c>
       <c r="J4">

</xml_diff>